<commit_message>
Fix error save ConditionalFormat DataBar
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/ConditionalFormatting/CFDataBarNegative.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/ConditionalFormatting/CFDataBarNegative.xlsx
@@ -372,30 +372,42 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:A4"/>
+  <x:dimension ref="A1:C4"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:1">
+    <x:row r="1" spans="1:3">
       <x:c r="A1" s="0" t="n">
         <x:v>-1</x:v>
       </x:c>
+      <x:c r="C1" s="0" t="n">
+        <x:v>-20</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:1">
+    <x:row r="2" spans="1:3">
       <x:c r="A2" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
+      <x:c r="C2" s="0" t="n">
+        <x:v>40</x:v>
+      </x:c>
     </x:row>
-    <x:row r="3" spans="1:1">
+    <x:row r="3" spans="1:3">
       <x:c r="A3" s="0" t="n">
         <x:v>2</x:v>
       </x:c>
+      <x:c r="C3" s="0" t="n">
+        <x:v>-60</x:v>
+      </x:c>
     </x:row>
-    <x:row r="4" spans="1:1">
+    <x:row r="4" spans="1:3">
       <x:c r="A4" s="0" t="n">
         <x:v>3</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="n">
+        <x:v>30</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -403,12 +415,26 @@
     <x:cfRule type="dataBar" priority="1">
       <x:dataBar showValue="1">
         <x:cfvo type="min" val="0"/>
-        <x:cfvo type="percent" val="100"/>
+        <x:cfvo type="max" val="0"/>
         <x:color rgb="FF008000"/>
       </x:dataBar>
       <x:extLst>
         <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{00000001-0000-0000-0000-000000000000}</x14:id>
+          <x14:id>{47cf17ea-008b-4284-87b7-63dbcafcbea5}</x14:id>
+        </x:ext>
+      </x:extLst>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="C1:C4">
+    <x:cfRule type="dataBar" priority="2">
+      <x:dataBar showValue="0">
+        <x:cfvo type="num" val="-100"/>
+        <x:cfvo type="num" val="100"/>
+        <x:color rgb="FF008000"/>
+      </x:dataBar>
+      <x:extLst>
+        <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{63c6ccc3-2167-4d97-8e9d-2c3ee4c3fc89}</x14:id>
         </x:ext>
       </x:extLst>
     </x:cfRule>
@@ -422,16 +448,35 @@
     <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{00000001-0000-0000-0000-000000000000}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0" axisPosition="middle">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
+          <x14:cfRule type="dataBar" id="{47cf17ea-008b-4284-87b7-63dbcafcbea5}">
+            <x14:dataBar minLength="0" maxLength="100" showValue="1" gradient="0" axisPosition="middle">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
               <x14:negativeFillColor rgb="FFFF0000"/>
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
           <xm:sqref>A1:A4</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{63c6ccc3-2167-4d97-8e9d-2c3ee4c3fc89}">
+            <x14:dataBar minLength="0" maxLength="100" showValue="0" gradient="0" axisPosition="middle">
+              <x14:cfvo type="num">
+                <xm:f>-100</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>100</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C1:C4</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </x:ext>
   </x:extLst>

</xml_diff>